<commit_message>
Ajustando para passar do captcha corretamente
</commit_message>
<xml_diff>
--- a/Consulta Multas.xlsx
+++ b/Consulta Multas.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandre.moura\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E1BF370-BB8D-469B-B8DC-17238F1300B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{271D0755-A4D9-4E0C-8CD7-FE9732460F11}"/>
+    <workbookView windowWidth="21000" windowHeight="7955"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,15 +14,15 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,6 +32,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
+    <t>PLACA</t>
+  </si>
+  <si>
+    <t>RENAVAM</t>
+  </si>
+  <si>
+    <t>CNPJ</t>
+  </si>
+  <si>
     <t>ESU6B64</t>
   </si>
   <si>
@@ -327,39 +330,373 @@
   </si>
   <si>
     <t>LUP8D66</t>
-  </si>
-  <si>
-    <t>PLACA</t>
-  </si>
-  <si>
-    <t>RENAVAN</t>
-  </si>
-  <si>
-    <t>CNPJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -367,9 +704,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -378,17 +957,61 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
+    <cellStyle name="Porcentagem" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moeda [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Hyperlink seguido" xfId="7" builtinId="9"/>
+    <cellStyle name="Observação" xfId="8" builtinId="10"/>
+    <cellStyle name="Texto de Aviso" xfId="9" builtinId="11"/>
+    <cellStyle name="Título" xfId="10" builtinId="15"/>
+    <cellStyle name="Texto Explicativo" xfId="11" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
+    <cellStyle name="Saída" xfId="17" builtinId="21"/>
+    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
+    <cellStyle name="Célula de Verificação" xfId="19" builtinId="23"/>
+    <cellStyle name="Célula Vinculada" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Bom" xfId="22" builtinId="26"/>
+    <cellStyle name="Ruim" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
+    <cellStyle name="Ênfase 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Ênfase 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Ênfase 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Ênfase 1" xfId="28" builtinId="32"/>
+    <cellStyle name="Ênfase 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Ênfase 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Ênfase 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Ênfase 2" xfId="32" builtinId="36"/>
+    <cellStyle name="Ênfase 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Ênfase 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Ênfase 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Ênfase 3" xfId="36" builtinId="40"/>
+    <cellStyle name="Ênfase 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Ênfase 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Ênfase 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Ênfase 4" xfId="40" builtinId="44"/>
+    <cellStyle name="Ênfase 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Ênfase 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Ênfase 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Ênfase 5" xfId="44" builtinId="48"/>
+    <cellStyle name="Ênfase 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Ênfase 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Ênfase 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -437,7 +1060,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -470,26 +1093,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -522,23 +1128,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -680,43 +1269,38 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA266B5-D25C-4E60-9E1A-C55599F541F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="17.8518518518519" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>329933248</v>
@@ -725,9 +1309,9 @@
         <v>15025071000116</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>329936441</v>
@@ -736,9 +1320,9 @@
         <v>15025071000116</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>329936735</v>
@@ -747,9 +1331,9 @@
         <v>15025071000116</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>329936913</v>
@@ -758,9 +1342,9 @@
         <v>41905203000104</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>1255425765</v>
@@ -769,9 +1353,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>1255433121</v>
@@ -780,9 +1364,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>1255921126</v>
@@ -791,9 +1375,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>1255921940</v>
@@ -802,9 +1386,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>1255922670</v>
@@ -813,9 +1397,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>1255923528</v>
@@ -824,9 +1408,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>1255924320</v>
@@ -835,9 +1419,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>1256656671</v>
@@ -846,9 +1430,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>1256660385</v>
@@ -857,9 +1441,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>1257631257</v>
@@ -868,9 +1452,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>1268122502</v>
@@ -879,9 +1463,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>1268151847</v>
@@ -890,9 +1474,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>1268157357</v>
@@ -901,9 +1485,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>1268160633</v>
@@ -912,9 +1496,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>1268161702</v>
@@ -923,9 +1507,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>1280873237</v>
@@ -934,9 +1518,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>1280876988</v>
@@ -945,9 +1529,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>1280877542</v>
@@ -956,9 +1540,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>1281181711</v>
@@ -967,9 +1551,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>1281182572</v>
@@ -978,9 +1562,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>1281912970</v>
@@ -989,9 +1573,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>1285247784</v>
@@ -1000,9 +1584,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>1285249094</v>
@@ -1011,9 +1595,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>1285249604</v>
@@ -1022,9 +1606,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>1285251412</v>
@@ -1033,9 +1617,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>1285252001</v>
@@ -1044,9 +1628,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>1285437648</v>
@@ -1055,9 +1639,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>1285440916</v>
@@ -1066,9 +1650,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>1302929990</v>
@@ -1077,9 +1661,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B35">
         <v>1304345880</v>
@@ -1088,9 +1672,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B36">
         <v>1304435706</v>
@@ -1099,9 +1683,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <v>1304436788</v>
@@ -1110,9 +1694,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>1317293700</v>
@@ -1121,9 +1705,9 @@
         <v>23373000001104</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>1317906893</v>
@@ -1132,9 +1716,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>1335692107</v>
@@ -1143,9 +1727,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>1336353977</v>
@@ -1154,9 +1738,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <v>1336376217</v>
@@ -1165,9 +1749,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B43">
         <v>142237930</v>
@@ -1176,9 +1760,9 @@
         <v>41905203000104</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B44">
         <v>888158556</v>
@@ -1187,9 +1771,9 @@
         <v>2373517000232</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B45">
         <v>1132614640</v>
@@ -1198,9 +1782,9 @@
         <v>15025071000116</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B46">
         <v>1132645287</v>
@@ -1209,9 +1793,9 @@
         <v>15025071000116</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B47">
         <v>1132615990</v>
@@ -1220,9 +1804,9 @@
         <v>41905203000104</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B48">
         <v>1181983514</v>
@@ -1231,9 +1815,9 @@
         <v>15025071000116</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B49">
         <v>1182384975</v>
@@ -1242,9 +1826,9 @@
         <v>15025071000116</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B50">
         <v>1189539508</v>
@@ -1253,9 +1837,9 @@
         <v>15025071000116</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B51">
         <v>1189542916</v>
@@ -1264,9 +1848,9 @@
         <v>15025071000116</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B52">
         <v>902672444</v>
@@ -1275,9 +1859,9 @@
         <v>2373517000232</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B53">
         <v>116468025</v>
@@ -1286,9 +1870,9 @@
         <v>23611642000122</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B54">
         <v>230317278</v>
@@ -1297,9 +1881,9 @@
         <v>41905203000104</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B55">
         <v>230318797</v>
@@ -1308,9 +1892,9 @@
         <v>41905203000104</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B56">
         <v>1234181891</v>
@@ -1319,9 +1903,9 @@
         <v>27893382000186</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B57">
         <v>1330087590</v>
@@ -1330,9 +1914,9 @@
         <v>23373000001104</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B58">
         <v>1330091709</v>
@@ -1341,9 +1925,9 @@
         <v>23373000001376</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B59">
         <v>1330092233</v>
@@ -1352,9 +1936,9 @@
         <v>23373000001104</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B60">
         <v>1330099521</v>
@@ -1363,9 +1947,9 @@
         <v>23373000001104</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B61">
         <v>1328194121</v>
@@ -1374,9 +1958,9 @@
         <v>23373000001104</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B62">
         <v>1231923277</v>
@@ -1385,9 +1969,9 @@
         <v>15025071000116</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B63">
         <v>1328189136</v>
@@ -1396,9 +1980,9 @@
         <v>23373000001105</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B64">
         <v>1028791620</v>
@@ -1407,9 +1991,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B65">
         <v>1029822198</v>
@@ -1418,9 +2002,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B66">
         <v>1029171731</v>
@@ -1429,9 +2013,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B67">
         <v>1029975512</v>
@@ -1440,9 +2024,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B68">
         <v>1070085372</v>
@@ -1451,9 +2035,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B69">
         <v>1110738975</v>
@@ -1462,9 +2046,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B70">
         <v>1110260382</v>
@@ -1473,9 +2057,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B71">
         <v>1122759735</v>
@@ -1484,9 +2068,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B72">
         <v>1122761055</v>
@@ -1495,9 +2079,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B73">
         <v>1070255227</v>
@@ -1506,9 +2090,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B74">
         <v>1111017368</v>
@@ -1517,9 +2101,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B75">
         <v>1155008542</v>
@@ -1528,9 +2112,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B76">
         <v>1155004113</v>
@@ -1539,9 +2123,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B77">
         <v>1185283592</v>
@@ -1550,9 +2134,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B78">
         <v>1185285986</v>
@@ -1561,9 +2145,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B79">
         <v>1191658284</v>
@@ -1572,9 +2156,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B80">
         <v>1189219759</v>
@@ -1583,9 +2167,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B81">
         <v>1189224507</v>
@@ -1594,9 +2178,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B82">
         <v>1029819049</v>
@@ -1605,9 +2189,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B83">
         <v>1062644376</v>
@@ -1616,9 +2200,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B84">
         <v>1070180375</v>
@@ -1627,9 +2211,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B85">
         <v>1110423737</v>
@@ -1638,9 +2222,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B86">
         <v>1125702068</v>
@@ -1649,9 +2233,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B87">
         <v>1125702947</v>
@@ -1660,9 +2244,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B88">
         <v>1122757600</v>
@@ -1671,9 +2255,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B89">
         <v>1155006388</v>
@@ -1682,9 +2266,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B90">
         <v>1155007341</v>
@@ -1693,9 +2277,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B91">
         <v>1155005659</v>
@@ -1704,9 +2288,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B92">
         <v>1184877790</v>
@@ -1715,9 +2299,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B93">
         <v>1189223110</v>
@@ -1726,9 +2310,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B94">
         <v>1193283032</v>
@@ -1737,9 +2321,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B95">
         <v>1193284373</v>
@@ -1748,9 +2332,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B96">
         <v>1191947219</v>
@@ -1759,9 +2343,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B97">
         <v>1191947413</v>
@@ -1770,9 +2354,9 @@
         <v>31437249000192</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B98">
         <v>1193287429</v>
@@ -1782,6 +2366,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>